<commit_message>
Fix csv and excel files
</commit_message>
<xml_diff>
--- a/resources/4_mei_encoding/AQUITANIANnotation-NClevel.xlsx
+++ b/resources/4_mei_encoding/AQUITANIANnotation-NClevel.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/OMR_Portuguese_Sources/resources/4_mei_encoding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EFC4CAA-5152-CF4C-AB9E-A32CE7C8E47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{78F849A4-D24F-C74F-90A6-546A784B6F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="46740" windowHeight="17440" xr2:uid="{0394C6CE-5AF9-CF4B-B63B-6BC72F9E9ED6}"/>
   </bookViews>
   <sheets>
     <sheet name="AQUITANIANnotation-NClevel" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -168,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="215" uniqueCount="91">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="106" uniqueCount="85">
   <si>
     <t>imagePath</t>
   </si>
@@ -271,9 +270,6 @@
 &lt;/neume&gt;</t>
   </si>
   <si>
-    <t>imageBinary</t>
-  </si>
-  <si>
     <t>https://pemdatabase.eu/iipsrv/iipsrv.fcgi?IIIF=images/1d335927-f461-4bdb-a6e5-069a24a9d3f1/RQKyrNTU8790.tiff/1478,2286,33,55/128,/0/default.jpg</t>
   </si>
   <si>
@@ -295,12 +291,6 @@
     <t>Dominus dabit, 1st line, benignitaTEM</t>
   </si>
   <si>
-    <t>&lt;neume&gt;</t>
-  </si>
-  <si>
-    <t>&lt;/neume&gt;</t>
-  </si>
-  <si>
     <t>https://pemdatabase.eu/iipsrv/iipsrv.fcgi?IIIF=images/1d335927-f461-4bdb-a6e5-069a24a9d3f1/s0N4NSFQ8805.tiff/1371,2130,50,37/128,/0/default.jpg</t>
   </si>
   <si>
@@ -334,36 +324,6 @@
     <t>neume.cephalicus</t>
   </si>
   <si>
-    <r>
-      <t>        </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF1F2328"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;liquescent/&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF1F2328"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/nc&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>https://pemdatabase.eu/iipsrv/iipsrv.fcgi?IIIF=images/1d335927-f461-4bdb-a6e5-069a24a9d3f1/oI017Xju8794.tiff/1847,720,60,65/128,/0/default.jpg</t>
   </si>
   <si>
@@ -455,21 +415,6 @@
   </si>
   <si>
     <t>neume.virgaliq</t>
-  </si>
-  <si>
-    <r>
-      <t>    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF1F2328"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;nc curve="c" tilt="ne"&gt;</t>
-    </r>
   </si>
   <si>
     <t>&lt;neume&gt;
@@ -525,7 +470,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -660,41 +605,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF1F2328"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF1F2328"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="16"/>
-      <color rgb="FF1F2328"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF1F2328"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -993,7 +903,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1036,21 +946,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1084,7 +987,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1551,8 +1453,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A001BD3-14A6-E347-AC0D-A7B160A0B128}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1607,7 +1509,7 @@
     </row>
     <row r="2" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" t="e" vm="1">
         <v>#VALUE!</v>
@@ -1616,10 +1518,10 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
         <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -1631,12 +1533,12 @@
         <v>13</v>
       </c>
       <c r="K2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="e" vm="2">
         <v>#VALUE!</v>
@@ -1645,10 +1547,10 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
         <v>35</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -1660,27 +1562,27 @@
         <v>16</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B4" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
         <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" t="s">
-        <v>43</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1689,12 +1591,12 @@
         <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B5" t="e" vm="4">
         <v>#VALUE!</v>
@@ -1703,10 +1605,10 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
@@ -1718,41 +1620,41 @@
         <v>20</v>
       </c>
       <c r="K5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B6" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="K6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B7" t="e" vm="6">
         <v>#VALUE!</v>
@@ -1761,10 +1663,10 @@
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
@@ -1773,15 +1675,15 @@
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B8" t="e" vm="7">
         <v>#VALUE!</v>
@@ -1790,10 +1692,10 @@
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
         <v>24</v>
@@ -1805,12 +1707,12 @@
         <v>25</v>
       </c>
       <c r="K8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B9" t="e" vm="8">
         <v>#VALUE!</v>
@@ -1819,10 +1721,10 @@
         <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
         <v>27</v>
@@ -1834,152 +1736,152 @@
         <v>28</v>
       </c>
       <c r="K9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B10" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="K10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B11" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B12" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F12" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="K12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B13" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F13" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B14" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="K14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1988,524 +1890,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7D97D6-9A66-0740-A0F3-BC2454B3DA9E}">
-  <dimension ref="A1:J18"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="127.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="3" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="5">
-        <v>1</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="3" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="5">
-        <v>1</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="3" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="3" t="e" vm="4">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="5">
-        <v>1</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="3" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="5">
-        <v>1</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="3" t="e" vm="6">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="3" t="e" vm="7">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="3" t="e" vm="8">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="3" t="e" vm="9">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="3" t="e" vm="10">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="3" t="e" vm="11">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="3" t="e" vm="12">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B14" s="3" t="e" vm="13">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G14" s="5">
-        <v>1</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{7E7316E7-D05B-744F-83AC-FF147E9B3DB6}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{91787C19-E206-0940-8426-BA4E8113BC90}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{735603B3-F186-1648-B22D-97429C238B05}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{6BB95BEF-9B4F-444B-9140-F53376DA9C63}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{6CA22B8F-5657-9C45-853F-429D247DD2D9}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{9942AF2D-D276-B443-8A5A-216354993B5F}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{74F9A618-AC96-9C41-8904-3A2412D75AE8}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{DA6FFAF4-C244-BE4F-8F67-6DD3158D202C}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{4BFDEBB7-4162-4944-9C51-44DCF43FBDA3}"/>
-    <hyperlink ref="A11" r:id="rId10" xr:uid="{D264C197-6788-7A42-9A1C-FEE038A8EB0E}"/>
-    <hyperlink ref="A12" r:id="rId11" xr:uid="{7C73B6BF-E67A-0C4B-A75D-BE7A4F5032F5}"/>
-    <hyperlink ref="A13" r:id="rId12" xr:uid="{26D139D6-13A0-1245-80C7-6CE0348E5274}"/>
-    <hyperlink ref="A14" r:id="rId13" xr:uid="{5F8092C0-EA08-8646-B69C-52CE983801F0}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix epiphonus in excel and csv files
</commit_message>
<xml_diff>
--- a/resources/4_mei_encoding/AQUITANIANnotation-NClevel.xlsx
+++ b/resources/4_mei_encoding/AQUITANIANnotation-NClevel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/OMR_Portuguese_Sources/resources/4_mei_encoding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{78F849A4-D24F-C74F-90A6-546A784B6F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5FBED1BC-E3BA-094B-96DC-A9405E123B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="46740" windowHeight="17440" xr2:uid="{0394C6CE-5AF9-CF4B-B63B-6BC72F9E9ED6}"/>
   </bookViews>
@@ -425,13 +425,6 @@
   </si>
   <si>
     <t>&lt;neume&gt;
-    &lt;nc curve="a" type="cephalicus"&gt;
-        &lt;liquescent/&gt;
-    &lt;/nc&gt;
-&lt;/neume&gt;</t>
-  </si>
-  <si>
-    <t>&lt;neume&gt;
     &lt;nc/&gt;
     &lt;nc intm="1S"/&gt;
     &lt;nc intm="-1S"/&gt;
@@ -461,6 +454,13 @@
   <si>
     <t>&lt;neume&gt;
     &lt;nc curve="c" tilt="ne"&gt;
+        &lt;liquescent/&gt;
+    &lt;/nc&gt;
+&lt;/neume&gt;</t>
+  </si>
+  <si>
+    <t>&lt;neume&gt;
+    &lt;nc curve="a" type="epiphonus"&gt;
         &lt;liquescent/&gt;
     &lt;/nc&gt;
 &lt;/neume&gt;</t>
@@ -1453,8 +1453,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A001BD3-14A6-E347-AC0D-A7B160A0B128}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1675,7 +1675,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="K7" t="s">
         <v>32</v>
@@ -1762,7 +1762,7 @@
         <v>59</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K10" t="s">
         <v>32</v>
@@ -1791,7 +1791,7 @@
         <v>59</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K11" t="s">
         <v>32</v>
@@ -1820,7 +1820,7 @@
         <v>59</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K12" t="s">
         <v>32</v>
@@ -1849,7 +1849,7 @@
         <v>59</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K13" t="s">
         <v>32</v>
@@ -1878,7 +1878,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K14" t="s">
         <v>32</v>

</xml_diff>